<commit_message>
Dowell Pin Qty updated
Number of Dowell Pin correted to 48 for printed WobbleX
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.6.xlsx
+++ b/bom/BOM_ZR_V2.6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{E7786C66-D7AF-4A3B-B8D1-655D717DAA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1776B4CB-3D81-4F45-8957-0E895C6CBAEE}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{E7786C66-D7AF-4A3B-B8D1-655D717DAA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{095B643D-C89D-49F2-8406-484FED36B90B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -995,25 +995,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1032,6 +1013,25 @@
         <scheme val="minor"/>
       </font>
       <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3555,10 +3555,10 @@
     <tableColumn id="6" xr3:uid="{0BCBCD91-246F-43A0-B8C5-04E596E69EEA}" name="Part Description" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{ACE43926-E340-4876-958D-0EF54DCBE9FA}" name="Make/Buy" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{DA7121B7-FA12-4C8D-991C-7770D7553E03}" name="QTY" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{91769ED2-A856-483D-B9EB-5FBE3739F558}" name="Included in kit?" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{F3D31371-2653-4B6C-8EF2-EBF3EDB7638C}" name="Comment" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{97C0D926-0B05-4BCC-BC0C-84F1540EE5F0}" name="Vendor" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{E5A8160D-7E28-49C9-8F1D-EB7E0F628E21}" name="Vendor URL" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{91769ED2-A856-483D-B9EB-5FBE3739F558}" name="Included in kit?" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{F3D31371-2653-4B6C-8EF2-EBF3EDB7638C}" name="Comment" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{97C0D926-0B05-4BCC-BC0C-84F1540EE5F0}" name="Vendor" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{E5A8160D-7E28-49C9-8F1D-EB7E0F628E21}" name="Vendor URL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3855,7 +3855,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A1:XFD39"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4070,7 +4070,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="7">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="I7" s="37" t="s">
         <v>169</v>

</xml_diff>

<commit_message>
ZR2.6 BOM Qty clarified
- ButtonHead M6 Screws Qty25 length should be 12mm not 14.
- Capscrew M4 Length should be 16mm, not 14.  Qty adjusted to 12.  (4 per ballscrew)
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.6.xlsx
+++ b/bom/BOM_ZR_V2.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{E7786C66-D7AF-4A3B-B8D1-655D717DAA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{095B643D-C89D-49F2-8406-484FED36B90B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7882F16C-C6A3-4689-A2C8-001CEB7FFDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="172">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Nut, T-Slot - M6 for 3030 profile</t>
   </si>
   <si>
-    <t>Screw, ButtonHead - M6X14mm</t>
-  </si>
-  <si>
     <t>M3X10_CapScrew_92290A115</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
   </si>
   <si>
     <t>Nut, Hex - M4</t>
-  </si>
-  <si>
-    <t>Screw, Cap - M4X14mm</t>
   </si>
   <si>
     <t>BedPlate</t>
@@ -622,6 +616,15 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>Screw, Cap - M4X16mm</t>
+  </si>
+  <si>
+    <t>Qty 4 per Ballscrews.  To attach WobbleX lower ring to the Ballscrew Nut</t>
+  </si>
+  <si>
+    <t>Screw, ButtonHead - M6X12mm</t>
   </si>
 </sst>
 </file>
@@ -3505,7 +3508,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1391479</xdr:colOff>
+      <xdr:colOff>1381954</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1175845</xdr:rowOff>
     </xdr:to>
@@ -3853,37 +3856,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="84.6" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="9"/>
-    <col min="2" max="2" width="16.453125" style="10"/>
-    <col min="3" max="3" width="16.453125" style="8"/>
-    <col min="4" max="4" width="20.7265625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="9"/>
+    <col min="2" max="2" width="16.42578125" style="10"/>
+    <col min="3" max="3" width="16.42578125" style="8"/>
+    <col min="4" max="4" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="44.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" style="12" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" style="7"/>
-    <col min="9" max="9" width="16.453125" style="37"/>
-    <col min="10" max="10" width="56.1796875" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="8"/>
-    <col min="12" max="12" width="39.81640625" style="11" customWidth="1"/>
-    <col min="13" max="16384" width="16.453125" style="5"/>
+    <col min="7" max="7" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" style="7"/>
+    <col min="9" max="9" width="16.42578125" style="37"/>
+    <col min="10" max="10" width="56.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="8"/>
+    <col min="12" max="12" width="39.85546875" style="11" customWidth="1"/>
+    <col min="13" max="16384" width="16.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -3892,19 +3895,19 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>3</v>
@@ -3913,9 +3916,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
@@ -3929,9 +3932,9 @@
       <c r="K2" s="16"/>
       <c r="L2" s="20"/>
     </row>
-    <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>5</v>
@@ -3940,10 +3943,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>5</v>
@@ -3952,21 +3955,21 @@
         <v>3</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K3" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L3" s="13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="26" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
@@ -3980,9 +3983,9 @@
       <c r="K4" s="16"/>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>6</v>
@@ -3991,10 +3994,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>6</v>
@@ -4003,21 +4006,21 @@
         <v>1</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L5" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>6</v>
@@ -4026,10 +4029,10 @@
         <v>3</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G6" s="22" t="s">
         <v>6</v>
@@ -4038,33 +4041,33 @@
         <v>2</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J6" s="31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="8">
         <v>4</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G7" s="22" t="s">
         <v>5</v>
@@ -4073,33 +4076,33 @@
         <v>48</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C8" s="8">
         <v>5</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>5</v>
@@ -4108,33 +4111,33 @@
         <v>12</v>
       </c>
       <c r="I8" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="8">
         <v>6</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>5</v>
@@ -4143,21 +4146,21 @@
         <v>12</v>
       </c>
       <c r="I9" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
@@ -4171,9 +4174,9 @@
       <c r="K10" s="16"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>5</v>
@@ -4182,10 +4185,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>5</v>
@@ -4194,15 +4197,15 @@
         <v>1</v>
       </c>
       <c r="I11" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>5</v>
@@ -4211,10 +4214,10 @@
         <v>8</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>5</v>
@@ -4223,15 +4226,15 @@
         <v>4</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="131" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="131.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>5</v>
@@ -4252,21 +4255,21 @@
         <v>3</v>
       </c>
       <c r="I13" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L13" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>5</v>
@@ -4275,10 +4278,10 @@
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>5</v>
@@ -4287,18 +4290,18 @@
         <v>3</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>5</v>
@@ -4307,10 +4310,10 @@
         <v>11</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>5</v>
@@ -4319,18 +4322,18 @@
         <v>3</v>
       </c>
       <c r="I15" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>5</v>
@@ -4339,10 +4342,10 @@
         <v>12</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>5</v>
@@ -4351,18 +4354,18 @@
         <v>3</v>
       </c>
       <c r="I16" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L16" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>5</v>
@@ -4374,7 +4377,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>5</v>
@@ -4383,18 +4386,18 @@
         <v>3</v>
       </c>
       <c r="I17" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>5</v>
@@ -4403,10 +4406,10 @@
         <v>14</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>5</v>
@@ -4415,12 +4418,12 @@
         <v>3</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>5</v>
@@ -4429,10 +4432,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>5</v>
@@ -4441,15 +4444,15 @@
         <v>3</v>
       </c>
       <c r="I19" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>5</v>
@@ -4458,10 +4461,10 @@
         <v>16</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>5</v>
@@ -4470,18 +4473,18 @@
         <v>1</v>
       </c>
       <c r="I20" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>5</v>
@@ -4490,10 +4493,10 @@
         <v>17</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>5</v>
@@ -4502,21 +4505,21 @@
         <v>3</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J21" s="31" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L21" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>5</v>
@@ -4525,10 +4528,10 @@
         <v>18</v>
       </c>
       <c r="E22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>5</v>
@@ -4537,27 +4540,27 @@
         <v>3</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" s="8">
         <v>19</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>26</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>27</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>5</v>
@@ -4566,53 +4569,53 @@
         <v>12</v>
       </c>
       <c r="I23" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="8">
         <v>20</v>
       </c>
       <c r="E24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I24" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J24" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="8">
         <v>21</v>
       </c>
       <c r="E25" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>19</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>20</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>5</v>
@@ -4621,24 +4624,24 @@
         <v>6</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="8">
         <v>22</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>5</v>
@@ -4647,27 +4650,27 @@
         <v>26</v>
       </c>
       <c r="I26" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="8">
         <v>23</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>5</v>
@@ -4676,27 +4679,27 @@
         <v>24</v>
       </c>
       <c r="I27" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J27" s="34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" s="8">
         <v>24</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>5</v>
@@ -4705,18 +4708,18 @@
         <v>6</v>
       </c>
       <c r="I28" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J28" s="31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8">
         <v>25</v>
@@ -4731,30 +4734,30 @@
         <v>5</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J29" s="31" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" s="8">
         <v>26</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>5</v>
@@ -4763,82 +4766,82 @@
         <v>26</v>
       </c>
       <c r="I30" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" s="8">
         <v>27</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J31" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C32" s="8">
         <v>28</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I32" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J32" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33" s="8">
         <v>29</v>
       </c>
       <c r="E33" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>5</v>
@@ -4847,15 +4850,15 @@
         <v>50</v>
       </c>
       <c r="I33" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="8">
         <v>30</v>
@@ -4873,24 +4876,24 @@
         <v>12</v>
       </c>
       <c r="I34" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" s="8">
         <v>31</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>5</v>
@@ -4899,108 +4902,111 @@
         <v>12</v>
       </c>
       <c r="I35" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" s="8">
         <v>32</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>30</v>
+        <v>169</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H36" s="7">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I36" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="J36" s="31" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C37" s="8">
         <v>33</v>
       </c>
       <c r="E37" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I37" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J37" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" s="8">
         <v>34</v>
       </c>
       <c r="E38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I38" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J38" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" s="8">
         <v>35</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>5</v>
@@ -5009,12 +5015,12 @@
         <v>4</v>
       </c>
       <c r="I39" s="37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>6</v>
@@ -5023,33 +5029,33 @@
         <v>36</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I40" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J40" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>6</v>
@@ -5058,10 +5064,10 @@
         <v>37</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>6</v>
@@ -5070,21 +5076,21 @@
         <v>1</v>
       </c>
       <c r="I41" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>6</v>
@@ -5093,33 +5099,33 @@
         <v>38</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I42" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>6</v>
@@ -5128,33 +5134,33 @@
         <v>39</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I43" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J43" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>6</v>
@@ -5163,10 +5169,10 @@
         <v>40</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>6</v>
@@ -5175,21 +5181,21 @@
         <v>1</v>
       </c>
       <c r="I44" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>6</v>
@@ -5198,33 +5204,33 @@
         <v>41</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I45" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J45" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K45" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>6</v>
@@ -5233,33 +5239,33 @@
         <v>42</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I46" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J46" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K46" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>6</v>
@@ -5268,10 +5274,10 @@
         <v>43</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>6</v>
@@ -5280,21 +5286,21 @@
         <v>1</v>
       </c>
       <c r="I47" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J47" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L47" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>6</v>
@@ -5303,33 +5309,33 @@
         <v>44</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H48" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I48" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J48" s="31" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L48" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>6</v>
@@ -5338,10 +5344,10 @@
         <v>45</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>6</v>
@@ -5350,18 +5356,18 @@
         <v>3</v>
       </c>
       <c r="I49" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L49" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>6</v>
@@ -5370,10 +5376,10 @@
         <v>46</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>6</v>
@@ -5382,21 +5388,21 @@
         <v>1</v>
       </c>
       <c r="I50" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J50" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L50" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>6</v>
@@ -5405,10 +5411,10 @@
         <v>47</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>6</v>
@@ -5417,21 +5423,21 @@
         <v>1</v>
       </c>
       <c r="I51" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J51" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L51" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>6</v>
@@ -5440,10 +5446,10 @@
         <v>48</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>6</v>
@@ -5452,21 +5458,21 @@
         <v>1</v>
       </c>
       <c r="I52" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J52" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L52" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>6</v>
@@ -5475,10 +5481,10 @@
         <v>49</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>6</v>
@@ -5487,21 +5493,21 @@
         <v>1</v>
       </c>
       <c r="I53" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J53" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L53" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>6</v>
@@ -5510,10 +5516,10 @@
         <v>50</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>6</v>
@@ -5522,21 +5528,21 @@
         <v>1</v>
       </c>
       <c r="I54" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J54" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L54" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>6</v>
@@ -5545,10 +5551,10 @@
         <v>51</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>6</v>
@@ -5557,21 +5563,21 @@
         <v>1</v>
       </c>
       <c r="I55" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J55" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L55" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>6</v>
@@ -5580,10 +5586,10 @@
         <v>52</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>6</v>
@@ -5592,21 +5598,21 @@
         <v>1</v>
       </c>
       <c r="I56" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J56" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L56" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>6</v>
@@ -5615,10 +5621,10 @@
         <v>53</v>
       </c>
       <c r="E57" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="12" t="s">
         <v>21</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>22</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>6</v>
@@ -5627,21 +5633,21 @@
         <v>3</v>
       </c>
       <c r="I57" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J57" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L57" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>6</v>
@@ -5650,10 +5656,10 @@
         <v>55</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>6</v>
@@ -5662,16 +5668,16 @@
         <v>2</v>
       </c>
       <c r="I58" s="37" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J58" s="31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L58" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5708,7 +5714,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
   <drawing r:id="rId28"/>
   <webPublishItems count="1">
-    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.6.htm" autoRepublish="1"/>
+    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\HevORT\bom\BOM_ZR_V2.6.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId29"/>

</xml_diff>

<commit_message>
Update to ZR2.6 BOM
- Added Qty 2 M5X16 Button head screws for ball screws top bearing mounts. RH + LH
- Added Z bed arm rodend support Qty 3 (same as ZR2.5) was missing in ZR2.6
Also ::
STLs for Bed plate support frame printed parts added to the ZR2.6 Folder.  Same parts as ZR2.5.
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.6.xlsx
+++ b/bom/BOM_ZR_V2.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EFA310-8053-4EA5-BC92-F5EF1071EB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF57564F-FD2D-4D54-96FB-8556D2E781DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" tabRatio="628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21820" tabRatio="628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="177">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -627,6 +627,21 @@
 Length determined by Frame Calculator:
 https://github.com/MirageC79/HevORT/tree/master/docs/assets/references/frame</t>
     </r>
+  </si>
+  <si>
+    <t>Z_Bed_Arm_RodEnd_Support</t>
+  </si>
+  <si>
+    <t>RodEnd_Support</t>
+  </si>
+  <si>
+    <t>M5X16_ButtonHeadScrew_91290A232</t>
+  </si>
+  <si>
+    <t>Screw, ButtonHead - M5X16mm</t>
+  </si>
+  <si>
+    <t>Qty 2 required for Ball Screw top bearing mount</t>
   </si>
 </sst>
 </file>
@@ -880,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -995,6 +1010,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1308,13 +1326,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1396,13 +1414,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1440,13 +1458,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1484,13 +1502,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1572,13 +1590,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1616,13 +1634,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1660,13 +1678,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1792,13 +1810,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1924,13 +1942,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2012,13 +2030,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2100,13 +2118,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2144,13 +2162,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2320,13 +2338,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2364,13 +2382,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2408,13 +2426,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2452,13 +2470,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2496,13 +2514,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>331148</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>288046</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1121586</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3024,13 +3042,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>104914</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>60740</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1336262</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>1248883</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3068,13 +3086,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>55217</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>60741</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1380435</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>1220307</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3112,13 +3130,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>115956</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>44174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1281043</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>1209261</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3156,13 +3174,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>104913</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1287125</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>1220304</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3200,13 +3218,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>138045</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1283593</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>1159565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3244,13 +3262,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>198783</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>71782</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1347305</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>1160172</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3288,13 +3306,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>204304</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>104914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1164389</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>1203740</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3332,13 +3350,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>182219</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>132523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1242393</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1192697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3376,13 +3394,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>132523</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>66261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1358349</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>1235597</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3420,13 +3438,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>88348</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>121478</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1258957</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>1100533</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3548,12 +3566,100 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>965200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82665AF2-C265-D73B-ED97-E7D152ABC693}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3663950" y="71132700"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>359088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1187450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1066800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="thumbnail_55.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3C46C0F-09B1-4A85-BDEA-7DA40D8EA1E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3683000" y="36808088"/>
+          <a:ext cx="952500" cy="707712"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C292BF5F-38F1-4DDC-8133-F36330D88A4B}" name="Table2" displayName="Table2" ref="A1:L58" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13">
-  <autoFilter ref="A1:L58" xr:uid="{F0C67E1A-5119-4B25-9FBC-2A59CD2F80D6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C292BF5F-38F1-4DDC-8133-F36330D88A4B}" name="Table2" displayName="Table2" ref="A1:L60" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:L60" xr:uid="{F0C67E1A-5119-4B25-9FBC-2A59CD2F80D6}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{371A3AB6-718E-44BA-A3CC-656ABDCDD768}" name="SubAssy" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{8D81458F-CC8E-4FB2-AC08-34D35D773E2C}" name="Category" dataDxfId="10"/>
@@ -3859,11 +3965,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3874,9 +3980,9 @@
     <col min="4" max="4" width="20.7265625" style="5" customWidth="1"/>
     <col min="5" max="5" width="44.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" style="12" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" style="7"/>
-    <col min="9" max="9" width="16.453125" style="37"/>
+    <col min="7" max="7" width="14.7265625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="19.26953125" style="37" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="56.1796875" style="31" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.453125" style="8"/>
     <col min="12" max="12" width="39.81640625" style="11" customWidth="1"/>
@@ -4720,7 +4826,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -4749,7 +4855,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -4775,7 +4881,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -4804,58 +4910,61 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C32" s="8">
-        <v>28</v>
+        <v>27.1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="7" t="s">
-        <v>105</v>
+      <c r="H32" s="7">
+        <v>2</v>
       </c>
       <c r="I32" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="J32" s="33" t="s">
-        <v>106</v>
+      <c r="J32" s="31" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="8">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="7">
-        <v>50</v>
+      <c r="H33" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="I33" s="37" t="s">
         <v>165</v>
+      </c>
+      <c r="J33" s="33" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4866,19 +4975,19 @@
         <v>69</v>
       </c>
       <c r="C34" s="8">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H34" s="7">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="I34" s="37" t="s">
         <v>165</v>
@@ -4892,13 +5001,13 @@
         <v>69</v>
       </c>
       <c r="C35" s="8">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>5</v>
@@ -4911,20 +5020,20 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="26" t="s">
-        <v>91</v>
+      <c r="A36" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C36" s="8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>5</v>
@@ -4935,37 +5044,34 @@
       <c r="I36" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="J36" s="31" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="28" t="s">
-        <v>85</v>
+      <c r="A37" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C37" s="8">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>15</v>
+        <v>166</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H37" s="7" t="s">
-        <v>109</v>
+      <c r="H37" s="7">
+        <v>12</v>
       </c>
       <c r="I37" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="J37" s="33" t="s">
-        <v>140</v>
+      <c r="J37" s="31" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4976,19 +5082,19 @@
         <v>69</v>
       </c>
       <c r="C38" s="8">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I38" s="37" t="s">
         <v>165</v>
@@ -4998,64 +5104,58 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="8">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="7">
-        <v>4</v>
+      <c r="H39" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="I39" s="37" t="s">
         <v>165</v>
       </c>
+      <c r="J39" s="33" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="26" t="s">
-        <v>91</v>
+      <c r="A40" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="C40" s="8">
+        <v>35</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>128</v>
-      </c>
       <c r="G40" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>109</v>
+        <v>5</v>
+      </c>
+      <c r="H40" s="7">
+        <v>4</v>
       </c>
       <c r="I40" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="J40" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="L40" s="13" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5066,25 +5166,25 @@
         <v>6</v>
       </c>
       <c r="C41" s="8">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="7">
-        <v>1</v>
+      <c r="H41" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="I41" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J41" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K41" s="8" t="s">
         <v>127</v>
@@ -5101,25 +5201,25 @@
         <v>6</v>
       </c>
       <c r="C42" s="8">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="7" t="s">
-        <v>109</v>
+      <c r="H42" s="7">
+        <v>1</v>
       </c>
       <c r="I42" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J42" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>127</v>
@@ -5136,13 +5236,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>6</v>
@@ -5171,25 +5271,25 @@
         <v>6</v>
       </c>
       <c r="C44" s="8">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="7">
-        <v>1</v>
+      <c r="H44" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="I44" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J44" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K44" s="8" t="s">
         <v>127</v>
@@ -5206,25 +5306,25 @@
         <v>6</v>
       </c>
       <c r="C45" s="8">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="7" t="s">
-        <v>109</v>
+      <c r="H45" s="7">
+        <v>1</v>
       </c>
       <c r="I45" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J45" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>127</v>
@@ -5241,13 +5341,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="8">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>6</v>
@@ -5276,25 +5376,25 @@
         <v>6</v>
       </c>
       <c r="C47" s="8">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H47" s="7">
-        <v>1</v>
+      <c r="H47" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="I47" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J47" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K47" s="8" t="s">
         <v>127</v>
@@ -5311,25 +5411,25 @@
         <v>6</v>
       </c>
       <c r="C48" s="8">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F48" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="7" t="s">
-        <v>109</v>
+      <c r="H48" s="7">
+        <v>1</v>
       </c>
       <c r="I48" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J48" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K48" s="8" t="s">
         <v>127</v>
@@ -5346,23 +5446,26 @@
         <v>6</v>
       </c>
       <c r="C49" s="8">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="F49" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H49" s="7">
-        <v>3</v>
+      <c r="H49" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="I49" s="37" t="s">
         <v>164</v>
       </c>
+      <c r="J49" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="K49" s="8" t="s">
         <v>127</v>
       </c>
@@ -5371,32 +5474,29 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
-        <v>85</v>
+      <c r="A50" s="26" t="s">
+        <v>91</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="8">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>55</v>
+        <v>137</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H50" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I50" s="37" t="s">
         <v>164</v>
-      </c>
-      <c r="J50" s="31" t="s">
-        <v>138</v>
       </c>
       <c r="K50" s="8" t="s">
         <v>127</v>
@@ -5413,13 +5513,13 @@
         <v>6</v>
       </c>
       <c r="C51" s="8">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F51" s="12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>6</v>
@@ -5448,13 +5548,13 @@
         <v>6</v>
       </c>
       <c r="C52" s="8">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>6</v>
@@ -5483,13 +5583,13 @@
         <v>6</v>
       </c>
       <c r="C53" s="8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>6</v>
@@ -5518,13 +5618,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="8">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>6</v>
@@ -5553,13 +5653,13 @@
         <v>6</v>
       </c>
       <c r="C55" s="8">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="G55" s="8" t="s">
         <v>6</v>
@@ -5588,13 +5688,13 @@
         <v>6</v>
       </c>
       <c r="C56" s="8">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="G56" s="8" t="s">
         <v>6</v>
@@ -5623,25 +5723,25 @@
         <v>6</v>
       </c>
       <c r="C57" s="8">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="G57" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H57" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I57" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J57" s="31" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="K57" s="8" t="s">
         <v>127</v>
@@ -5650,7 +5750,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="14" t="s">
         <v>85</v>
       </c>
@@ -5658,30 +5758,100 @@
         <v>6</v>
       </c>
       <c r="C58" s="8">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>22</v>
+        <v>172</v>
       </c>
       <c r="F58" s="12" t="s">
-        <v>22</v>
+        <v>173</v>
       </c>
       <c r="G58" s="8" t="s">
         <v>6</v>
       </c>
       <c r="H58" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I58" s="37" t="s">
         <v>164</v>
       </c>
       <c r="J58" s="31" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="K58" s="8" t="s">
         <v>127</v>
       </c>
       <c r="L58" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="8">
+        <v>54</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="7">
+        <v>3</v>
+      </c>
+      <c r="I59" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="J59" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="L59" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="8">
+        <v>55</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="7">
+        <v>2</v>
+      </c>
+      <c r="I60" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="J60" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="L60" s="13" t="s">
         <v>99</v>
       </c>
     </row>
@@ -5692,37 +5862,38 @@
     <hyperlink ref="L3" r:id="rId2" xr:uid="{F3EDD62A-3F23-470A-B109-F73FF8D7C73C}"/>
     <hyperlink ref="L5" r:id="rId3" xr:uid="{50FB8D51-362E-4606-8D6E-8D956A41ECF5}"/>
     <hyperlink ref="L6" r:id="rId4" xr:uid="{2F73B2AD-698B-4466-8588-D83734F2C51B}"/>
-    <hyperlink ref="L40" r:id="rId5" xr:uid="{7D092ACD-881E-47AD-9B3B-4C449D63D40F}"/>
-    <hyperlink ref="L41" r:id="rId6" xr:uid="{407162CC-4C29-4D0C-91DC-B655A8620F0B}"/>
-    <hyperlink ref="L42" r:id="rId7" xr:uid="{AADA7E44-6402-4D18-9204-8FF05E003D4D}"/>
-    <hyperlink ref="L43" r:id="rId8" xr:uid="{0A6F950B-C88D-4A44-9046-4D13F81E37E0}"/>
-    <hyperlink ref="L44" r:id="rId9" xr:uid="{516A6813-7AFA-4F99-9E56-F3E3B09566BA}"/>
-    <hyperlink ref="L45" r:id="rId10" xr:uid="{AFDC888D-2FD9-4632-863B-A5C17D9F0E11}"/>
-    <hyperlink ref="L46" r:id="rId11" xr:uid="{F25CDF66-684F-42C1-984A-22FA54F1FD6C}"/>
-    <hyperlink ref="L47" r:id="rId12" xr:uid="{B7843521-AA6E-4400-A32E-88EDDECE67D9}"/>
-    <hyperlink ref="L48" r:id="rId13" xr:uid="{7E347213-2075-43D0-AD04-B1E1E6CCD53D}"/>
-    <hyperlink ref="L49" r:id="rId14" xr:uid="{56678C8C-8EC1-4CD9-9B3B-E21DFCC2978F}"/>
-    <hyperlink ref="L50" r:id="rId15" xr:uid="{6F13A277-23A7-41C3-A4F9-2EAFC1049FD4}"/>
-    <hyperlink ref="L51" r:id="rId16" xr:uid="{E3446744-430B-413E-BC36-EB62061E8825}"/>
-    <hyperlink ref="L52" r:id="rId17" xr:uid="{E660FC95-A247-4F95-B40B-D49B17698DF6}"/>
-    <hyperlink ref="L53" r:id="rId18" xr:uid="{AB4FB2F4-C13D-4AAF-BB6A-95B03DE5B521}"/>
-    <hyperlink ref="L54" r:id="rId19" xr:uid="{CD08D4C0-4E3F-45E5-A329-CBF47F8FAB76}"/>
-    <hyperlink ref="L55" r:id="rId20" xr:uid="{D2FE54E5-87A0-4B3D-B2E0-90E464696FF2}"/>
-    <hyperlink ref="L56" r:id="rId21" xr:uid="{D6C86378-B35E-4886-A088-31B005C533AA}"/>
-    <hyperlink ref="L57" r:id="rId22" xr:uid="{3C1179F3-53A3-495A-9742-6BE7C28D2E2A}"/>
-    <hyperlink ref="L58" r:id="rId23" xr:uid="{A34DF9FE-AE55-4AEC-9F63-92431BC31329}"/>
+    <hyperlink ref="L41" r:id="rId5" xr:uid="{7D092ACD-881E-47AD-9B3B-4C449D63D40F}"/>
+    <hyperlink ref="L42" r:id="rId6" xr:uid="{407162CC-4C29-4D0C-91DC-B655A8620F0B}"/>
+    <hyperlink ref="L43" r:id="rId7" xr:uid="{AADA7E44-6402-4D18-9204-8FF05E003D4D}"/>
+    <hyperlink ref="L44" r:id="rId8" xr:uid="{0A6F950B-C88D-4A44-9046-4D13F81E37E0}"/>
+    <hyperlink ref="L45" r:id="rId9" xr:uid="{516A6813-7AFA-4F99-9E56-F3E3B09566BA}"/>
+    <hyperlink ref="L46" r:id="rId10" xr:uid="{AFDC888D-2FD9-4632-863B-A5C17D9F0E11}"/>
+    <hyperlink ref="L47" r:id="rId11" xr:uid="{F25CDF66-684F-42C1-984A-22FA54F1FD6C}"/>
+    <hyperlink ref="L48" r:id="rId12" xr:uid="{B7843521-AA6E-4400-A32E-88EDDECE67D9}"/>
+    <hyperlink ref="L49" r:id="rId13" xr:uid="{7E347213-2075-43D0-AD04-B1E1E6CCD53D}"/>
+    <hyperlink ref="L50" r:id="rId14" xr:uid="{56678C8C-8EC1-4CD9-9B3B-E21DFCC2978F}"/>
+    <hyperlink ref="L51" r:id="rId15" xr:uid="{6F13A277-23A7-41C3-A4F9-2EAFC1049FD4}"/>
+    <hyperlink ref="L52" r:id="rId16" xr:uid="{E3446744-430B-413E-BC36-EB62061E8825}"/>
+    <hyperlink ref="L53" r:id="rId17" xr:uid="{E660FC95-A247-4F95-B40B-D49B17698DF6}"/>
+    <hyperlink ref="L54" r:id="rId18" xr:uid="{AB4FB2F4-C13D-4AAF-BB6A-95B03DE5B521}"/>
+    <hyperlink ref="L55" r:id="rId19" xr:uid="{CD08D4C0-4E3F-45E5-A329-CBF47F8FAB76}"/>
+    <hyperlink ref="L56" r:id="rId20" xr:uid="{D2FE54E5-87A0-4B3D-B2E0-90E464696FF2}"/>
+    <hyperlink ref="L57" r:id="rId21" xr:uid="{D6C86378-B35E-4886-A088-31B005C533AA}"/>
+    <hyperlink ref="L59" r:id="rId22" xr:uid="{3C1179F3-53A3-495A-9742-6BE7C28D2E2A}"/>
+    <hyperlink ref="L60" r:id="rId23" xr:uid="{A34DF9FE-AE55-4AEC-9F63-92431BC31329}"/>
     <hyperlink ref="L15" r:id="rId24" xr:uid="{635A990E-4C95-4DEC-8B43-E601D8DDFF41}"/>
     <hyperlink ref="L13" r:id="rId25" xr:uid="{D31D20CB-B364-4F9C-B7F2-3002804FA790}"/>
     <hyperlink ref="L14" r:id="rId26" xr:uid="{92843DE4-0768-40BF-8533-757097709C78}"/>
+    <hyperlink ref="L58" r:id="rId27" xr:uid="{7B0AAD1E-7BAB-4965-8D01-2F29B3EB5879}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
-  <drawing r:id="rId28"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
+  <drawing r:id="rId29"/>
   <webPublishItems count="1">
     <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\HevORT\bom\BOM_ZR_V2.6.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>